<commit_message>
Riktig dato for datauttak motorveg
</commit_message>
<xml_diff>
--- a/kostraleveranse2023/Kostra 02 - Fylkesveg med motorveg og motortrafikkveg.xlsx
+++ b/kostraleveranse2023/Kostra 02 - Fylkesveg med motorveg og motortrafikkveg.xlsx
@@ -545,7 +545,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-01-02</t>
+          <t>2024-01-09</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-12-31</t>
         </is>
       </c>
     </row>

</xml_diff>